<commit_message>
GPLIM-3541: add Material Type as required header for Manifest uploads
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/manifest-import/headers-only.xlsx
+++ b/mercury/src/test/resources/testdata/manifest-import/headers-only.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Specimen_Number</t>
   </si>
@@ -37,13 +37,16 @@
   </si>
   <si>
     <t>SAMPLE_TYPE</t>
+  </si>
+  <si>
+    <t>Material Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -64,6 +67,10 @@
       <color theme="0"/>
       <name val="MS Sans Serif"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
     </font>
   </fonts>
   <fills count="5">
@@ -104,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -113,6 +120,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -446,15 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,6 +483,78 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="7:7">
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="7:7">
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="7:7">
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="7:7">
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="7:7">
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="7:7">
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="7:7">
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="7:7">
+      <c r="G24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>